<commit_message>
[body state]update my physical status today
</commit_message>
<xml_diff>
--- a/Personal/xueyu/身体状态记录.xlsx
+++ b/Personal/xueyu/身体状态记录.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="身体状态" sheetId="7" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="171027"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -83,8 +83,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,21 +156,21 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -186,8 +186,18 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -215,7 +225,7 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -224,10 +234,12 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="3"/>
           <c:order val="0"/>
@@ -242,17 +254,41 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>身体状态!$A$2:$A$23</c:f>
               <c:numCache>
-                <c:formatCode>yyyy/m/d</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>43136</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>43137</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43138</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -269,14 +305,29 @@
                 <c:pt idx="1">
                   <c:v>6</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-28CA-47A6-B8D8-3FE9652FF6B7}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="62844288"/>
         <c:axId val="63124992"/>
       </c:lineChart>
@@ -285,6 +336,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -312,7 +364,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -321,8 +373,9 @@
             <a:effectLst/>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="yyyy/m/d" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -361,12 +414,14 @@
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
         <c:axId val="63124992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -408,7 +463,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -419,6 +474,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -467,7 +523,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -496,7 +552,9 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="0"/>
     <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -556,7 +614,7 @@
         <xdr:cNvPr id="3" name="图表 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{038A3D36-3399-4C22-8358-33970E9B14AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{038A3D36-3399-4C22-8358-33970E9B14AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -578,10 +636,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="B1:B23" totalsRowCount="1" headerRowDxfId="4" dataDxfId="3" totalsRowDxfId="2">
-  <autoFilter ref="B1:B22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表2_2" displayName="表2_2" ref="B1:B23" totalsRowCount="1" headerRowDxfId="4" dataDxfId="3" totalsRowDxfId="2">
+  <autoFilter ref="B1:B22" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="1">
-    <tableColumn id="4" name="xy" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="xy" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -842,21 +900,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="X25" sqref="X25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.125" style="3" customWidth="1"/>
     <col min="2" max="2" width="12.75" style="3" customWidth="1"/>
@@ -865,7 +923,7 @@
     <col min="8" max="8" width="5.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -873,7 +931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>43136</v>
       </c>
@@ -881,7 +939,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>43137</v>
       </c>
@@ -889,94 +947,98 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="4"/>
-    </row>
-    <row r="5" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>43138</v>
+      </c>
+      <c r="B4" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="4"/>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B23" s="3">
-        <f>SUBTOTAL(109,[xy])</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
+        <f>SUBTOTAL(109,表2_2[xy])</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>0</v>
       </c>
@@ -984,7 +1046,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>1</v>
       </c>
@@ -992,7 +1054,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>2</v>
       </c>
@@ -1009,7 +1071,7 @@
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>3</v>
       </c>
@@ -1017,7 +1079,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>4</v>
       </c>
@@ -1025,7 +1087,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>5</v>
       </c>
@@ -1033,7 +1095,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>6</v>
       </c>
@@ -1041,7 +1103,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>7</v>
       </c>
@@ -1049,7 +1111,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>8</v>
       </c>
@@ -1057,7 +1119,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>9</v>
       </c>
@@ -1065,7 +1127,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
[physical status] update my physical status
</commit_message>
<xml_diff>
--- a/Personal/xueyu/身体状态记录.xlsx
+++ b/Personal/xueyu/身体状态记录.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4506"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="身体状态" sheetId="7" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>xy</t>
   </si>
@@ -77,14 +77,22 @@
   </si>
   <si>
     <t>旨在找到自己身体什么时候更疲劳，怀疑自己的身体像月经一样有规律</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>眼睛和颈部累</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>说明</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,23 +162,30 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="7">
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -186,18 +201,8 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="zh-CN"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -225,7 +230,7 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -234,12 +239,10 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="stacked"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="3"/>
           <c:order val="0"/>
@@ -262,14 +265,8 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -279,7 +276,7 @@
             <c:numRef>
               <c:f>身体状态!$A$2:$A$23</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>yyyy/m/d</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>43136</c:v>
@@ -289,6 +286,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>43138</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43139</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -308,35 +308,30 @@
                 <c:pt idx="2">
                   <c:v>4</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-28CA-47A6-B8D8-3FE9652FF6B7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="62844288"/>
-        <c:axId val="63124992"/>
+        <c:axId val="73478144"/>
+        <c:axId val="73480064"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="62844288"/>
+        <c:axId val="73478144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -364,7 +359,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -373,9 +368,8 @@
             <a:effectLst/>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="yyyy/m/d" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -410,18 +404,17 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63124992"/>
+        <c:crossAx val="73480064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="63124992"/>
+        <c:axId val="73480064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -463,7 +456,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -474,7 +467,6 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -509,7 +501,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62844288"/>
+        <c:crossAx val="73478144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -523,7 +515,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -552,9 +544,7 @@
         </a:p>
       </c:txPr>
     </c:legend>
-    <c:plotVisOnly val="0"/>
     <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -588,7 +578,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -598,23 +588,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>476252</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>276227</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="图表 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{038A3D36-3399-4C22-8358-33970E9B14AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{038A3D36-3399-4C22-8358-33970E9B14AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -636,10 +626,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表2_2" displayName="表2_2" ref="B1:B23" totalsRowCount="1" headerRowDxfId="4" dataDxfId="3" totalsRowDxfId="2">
-  <autoFilter ref="B1:B22" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="1">
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="xy" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="B1:C23" totalsRowCount="1" headerRowDxfId="6" dataDxfId="5" totalsRowDxfId="4">
+  <autoFilter ref="B1:C22">
+    <filterColumn colId="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="4" name="xy" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="1"/>
+    <tableColumn id="1" name="说明" dataDxfId="2" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -900,145 +893,177 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X25" sqref="X25"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="12.125" style="3" customWidth="1"/>
     <col min="2" max="2" width="12.75" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.25" customWidth="1"/>
     <col min="5" max="6" width="6.125" customWidth="1"/>
     <col min="7" max="7" width="18.75" customWidth="1"/>
     <col min="8" max="8" width="5.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2">
         <v>43136</v>
       </c>
       <c r="B2" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2">
         <v>43137</v>
       </c>
       <c r="B3" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="2">
         <v>43138</v>
       </c>
       <c r="B4" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2">
+        <v>43139</v>
+      </c>
+      <c r="B5" s="4">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="2"/>
       <c r="B6" s="4"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="2"/>
       <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="2"/>
       <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="2"/>
       <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="2"/>
       <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="2"/>
       <c r="B12" s="4"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="2"/>
       <c r="B13" s="4"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="2"/>
       <c r="B17" s="4"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="2"/>
       <c r="B18" s="4"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="2"/>
       <c r="B19" s="4"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="2"/>
       <c r="B20" s="4"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="2"/>
       <c r="B21" s="4"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="2"/>
       <c r="B22" s="4"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23" spans="1:11">
       <c r="B23" s="3">
-        <f>SUBTOTAL(109,表2_2[xy])</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+        <f>SUBTOTAL(109,[xy])</f>
+        <v>20</v>
+      </c>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11">
       <c r="A29" s="3">
         <v>0</v>
       </c>
@@ -1046,7 +1071,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11">
       <c r="A30" s="3">
         <v>1</v>
       </c>
@@ -1054,7 +1079,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11">
       <c r="A31" s="3">
         <v>2</v>
       </c>
@@ -1071,7 +1096,7 @@
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11">
       <c r="A32" s="3">
         <v>3</v>
       </c>
@@ -1079,7 +1104,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2">
       <c r="A33" s="3">
         <v>4</v>
       </c>
@@ -1087,7 +1112,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2">
       <c r="A34" s="3">
         <v>5</v>
       </c>
@@ -1095,7 +1120,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2">
       <c r="A35" s="3">
         <v>6</v>
       </c>
@@ -1103,7 +1128,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2">
       <c r="A36" s="3">
         <v>7</v>
       </c>
@@ -1111,7 +1136,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2">
       <c r="A37" s="3">
         <v>8</v>
       </c>
@@ -1119,7 +1144,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2">
       <c r="A38" s="3">
         <v>9</v>
       </c>
@@ -1127,7 +1152,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2">
       <c r="A39" s="3">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
[physical status] update my status, the body is so tired
</commit_message>
<xml_diff>
--- a/Personal/xueyu/身体状态记录.xlsx
+++ b/Personal/xueyu/身体状态记录.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="身体状态" sheetId="7" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="171027"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>xy</t>
   </si>
@@ -85,14 +85,18 @@
   </si>
   <si>
     <t>说明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>身体很累</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,28 +168,28 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -201,8 +205,18 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -230,7 +244,7 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -239,10 +253,12 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="3"/>
           <c:order val="0"/>
@@ -265,8 +281,14 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -276,7 +298,7 @@
             <c:numRef>
               <c:f>身体状态!$A$2:$A$23</c:f>
               <c:numCache>
-                <c:formatCode>yyyy/m/d</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>43136</c:v>
@@ -289,6 +311,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>43139</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43140</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -311,19 +336,29 @@
                 <c:pt idx="3">
                   <c:v>6</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:smooth val="0"/>
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-28CA-47A6-B8D8-3FE9652FF6B7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="73478144"/>
         <c:axId val="73480064"/>
       </c:lineChart>
@@ -332,6 +367,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -359,7 +395,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -368,8 +404,9 @@
             <a:effectLst/>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="yyyy/m/d" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -415,6 +452,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -456,7 +494,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -467,6 +505,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -515,7 +554,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -544,7 +583,9 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="0"/>
     <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -604,7 +645,7 @@
         <xdr:cNvPr id="3" name="图表 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{038A3D36-3399-4C22-8358-33970E9B14AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{038A3D36-3399-4C22-8358-33970E9B14AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -626,13 +667,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="B1:C23" totalsRowCount="1" headerRowDxfId="6" dataDxfId="5" totalsRowDxfId="4">
-  <autoFilter ref="B1:C22">
-    <filterColumn colId="1"/>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表2_2" displayName="表2_2" ref="B1:C23" totalsRowCount="1" headerRowDxfId="6" dataDxfId="5" totalsRowDxfId="4">
+  <autoFilter ref="B1:C22" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
-    <tableColumn id="4" name="xy" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="1"/>
-    <tableColumn id="1" name="说明" dataDxfId="2" totalsRowDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="xy" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="说明" dataDxfId="2" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -893,21 +932,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.125" style="3" customWidth="1"/>
     <col min="2" max="2" width="12.75" style="3" customWidth="1"/>
@@ -917,7 +956,7 @@
     <col min="8" max="8" width="5.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -928,7 +967,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>43136</v>
       </c>
@@ -937,7 +976,7 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>43137</v>
       </c>
@@ -946,7 +985,7 @@
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>43138</v>
       </c>
@@ -955,7 +994,7 @@
       </c>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>43139</v>
       </c>
@@ -966,104 +1005,110 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>43140</v>
+      </c>
+      <c r="B6" s="4">
+        <v>7</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B23" s="3">
-        <f>SUBTOTAL(109,[xy])</f>
-        <v>20</v>
+        <f>SUBTOTAL(109,表2_2[xy])</f>
+        <v>27</v>
       </c>
       <c r="C23" s="3"/>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>0</v>
       </c>
@@ -1071,7 +1116,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>1</v>
       </c>
@@ -1079,7 +1124,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>2</v>
       </c>
@@ -1096,7 +1141,7 @@
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>3</v>
       </c>
@@ -1104,7 +1149,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>4</v>
       </c>
@@ -1112,7 +1157,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>5</v>
       </c>
@@ -1120,7 +1165,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>6</v>
       </c>
@@ -1128,7 +1173,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>7</v>
       </c>
@@ -1136,7 +1181,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>8</v>
       </c>
@@ -1144,7 +1189,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>9</v>
       </c>
@@ -1152,7 +1197,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>10</v>
       </c>

</xml_diff>